<commit_message>
Update logo and sample config
</commit_message>
<xml_diff>
--- a/assets/sample-config.xlsx
+++ b/assets/sample-config.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -97,10 +97,13 @@
     <t xml:space="preserve">body-fields</t>
   </si>
   <si>
+    <t xml:space="preserve">[data.field, data.something]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">header-fields</t>
+  </si>
+  <si>
     <t xml:space="preserve">[]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">header-fields</t>
   </si>
   <si>
     <t xml:space="preserve">google</t>
@@ -359,7 +362,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F3" activeCellId="0" sqref="F3"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -454,7 +457,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -501,7 +504,7 @@
         <v>25</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -539,7 +542,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,7 +550,7 @@
         <v>19</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -555,7 +558,7 @@
         <v>21</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -593,7 +596,7 @@
         <v>17</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -601,15 +604,15 @@
         <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix excel loader and vendor expected tag value
</commit_message>
<xml_diff>
--- a/assets/sample-config.xlsx
+++ b/assets/sample-config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="pages" sheetId="1" state="visible" r:id="rId3"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -31,9 +31,6 @@
     <t xml:space="preserve">target-url</t>
   </si>
   <si>
-    <t xml:space="preserve">expected-destination</t>
-  </si>
-  <si>
     <t xml:space="preserve">vendors</t>
   </si>
   <si>
@@ -53,9 +50,6 @@
   </si>
   <si>
     <t xml:space="preserve">auto</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.usaa.com/auto</t>
   </si>
   <si>
     <t xml:space="preserve">https://www.usaa.com/inet/wc/auto-insurance?vurl=VURL_auto</t>
@@ -139,6 +133,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -160,17 +155,20 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -215,24 +213,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,85 +361,77 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="53.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="12.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="18.17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="10.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="5.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="53.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="12.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="18.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.06"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="E2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="F2" s="1" t="n">
+        <v>1244998375585961</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="0" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="0" t="n">
-        <v>1244998375585961</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I2" s="0" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://www.usaa.com/auto"/>
-    <hyperlink ref="C2" r:id="rId2" display="https://www.usaa.com/inet/wc/auto-insurance?vurl=VURL_auto"/>
+    <hyperlink ref="B2" r:id="rId1" display="https://www.usaa.com/inet/wc/auto-insurance?vurl=VURL_auto"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -456,55 +450,55 @@
   </sheetPr>
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.17"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="12.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.77"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="18.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B2" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -534,31 +528,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="25.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="25.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B2" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -588,31 +582,31 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="18.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B2" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="4" t="s">
+      <c r="B3" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>